<commit_message>
combined upload actually working
</commit_message>
<xml_diff>
--- a/test/templates/template_combined.xlsx
+++ b/test/templates/template_combined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flashton/Dropbox/scripts/seqbox/test/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31882798-9A9D-8443-A42C-420087C9961F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9CAA7B-3F4D-1B4B-B982-2D2D458C3F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{A4746E25-F57C-A545-A491-8E3F5F46AFEF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="91">
   <si>
     <t>sample_identifier</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t>barcode04</t>
+  </si>
+  <si>
+    <t>]</t>
   </si>
 </sst>
 </file>
@@ -708,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05DC6CF4-2BA4-1D46-B587-F3FC146B4466}">
-  <dimension ref="A1:AK13"/>
+  <dimension ref="A1:AK14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AI14" sqref="AI14"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1713,6 +1716,11 @@
     <row r="13" spans="1:37" x14ac:dyDescent="0.2">
       <c r="AA13" s="1"/>
     </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI14" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>